<commit_message>
Corrected a couple of minor errors in the v5 example s/sheets
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/filled/Example_v5.0.0_spreadsheet.xlsx
+++ b/examples/spreadsheets/v5/filled/Example_v5.0.0_spreadsheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwelter/Development/HCA/metadata-schema/examples/spreadsheets/v5/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="1540" windowWidth="35480" windowHeight="21700" activeTab="3"/>
+    <workbookView xWindow="15160" yWindow="460" windowWidth="19160" windowHeight="23540" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="286">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -848,9 +848,6 @@
     <t>smart-seq2</t>
   </si>
   <si>
-    <t>five_prime_end</t>
-  </si>
-  <si>
     <t>unstranded</t>
   </si>
   <si>
@@ -896,7 +893,7 @@
     <t>read2</t>
   </si>
   <si>
-    <t>astrocyte</t>
+    <t>5 prime end bias</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1484,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s">
         <v>282</v>
-      </c>
-      <c r="B4" t="s">
-        <v>283</v>
       </c>
       <c r="D4" t="s">
         <v>241</v>
@@ -1502,18 +1499,18 @@
         <v>263</v>
       </c>
       <c r="G4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5" t="s">
         <v>284</v>
-      </c>
-      <c r="B5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D5" t="s">
-        <v>285</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1522,7 +1519,7 @@
         <v>263</v>
       </c>
       <c r="G5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -1981,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2213,9 +2210,6 @@
         <v>258</v>
       </c>
       <c r="M4" t="s">
-        <v>286</v>
-      </c>
-      <c r="N4" t="s">
         <v>259</v>
       </c>
       <c r="X4" s="5" t="s">
@@ -2232,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2470,7 +2464,7 @@
         <v>260</v>
       </c>
       <c r="Z4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2483,7 +2477,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2594,7 +2588,7 @@
         <v>265</v>
       </c>
       <c r="J4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2606,8 +2600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2820,19 +2814,19 @@
         <v>268</v>
       </c>
       <c r="K4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L4" t="s">
         <v>269</v>
       </c>
       <c r="M4" t="s">
+        <v>285</v>
+      </c>
+      <c r="O4" t="s">
         <v>270</v>
       </c>
-      <c r="O4" t="s">
-        <v>271</v>
-      </c>
       <c r="W4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2971,19 +2965,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I4" t="s">
         <v>255</v>
       </c>
       <c r="M4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -3072,7 +3066,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>225</v>
@@ -3080,18 +3074,18 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>